<commit_message>
fix bug in total cost
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: -3,2)</t>
+          <t>(203957296, Omri Ben Shabat: 5,-2)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: -2,1)</t>
+          <t>(206532695, Matan Vakrat: -7,7)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -10,-9)</t>
+          <t>(302962915, Asher  Odeh: -1,9)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: -3,0)</t>
+          <t>(308035542, Anastasia  Kubi: -6,2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: -4,-1)</t>
+          <t>(311177802, Christina  Uksusman: 0,9)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -10,1)</t>
+          <t>(305251175, Or  Leder: -4,1)</t>
         </is>
       </c>
     </row>
@@ -463,14 +463,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 454.77753490851046</t>
+          <t>cost: 409.72557563737143</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 41.2221918635638</t>
+          <t>time: 48.09069695467143</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
create time matrix - in progress
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: 5,-2)</t>
+          <t>(203957296, Omri Ben Shabat: -5,6)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: -7,7)</t>
+          <t>(206532695, Matan Vakrat: -9,-9)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -1,9)</t>
+          <t>(302962915, Asher  Odeh: -10,1)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: -6,2)</t>
+          <t>(308035542, Anastasia  Kubi: 7,2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: 0,9)</t>
+          <t>(311177802, Christina  Uksusman: 2,-2)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -4,1)</t>
+          <t>(305251175, Or  Leder: 3,-9)</t>
         </is>
       </c>
     </row>
@@ -463,18 +463,18 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 409.72557563737143</t>
+          <t>cost: 596.4148259012275</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 48.09069695467143</t>
+          <t>time: 71.42685323765343</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create time travel matrix
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: -2,-9)</t>
+          <t>(203957296, Omri Ben Shabat: 7,8)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: 8,-6)</t>
+          <t>(206532695, Matan Vakrat: -8,5)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -7,-10)</t>
+          <t>(302962915, Asher  Odeh: -8,-8)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: -8,3)</t>
+          <t>(308035542, Anastasia  Kubi: 6,-2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: -8,5)</t>
+          <t>(311177802, Christina  Uksusman: -7,-7)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -7,-7)</t>
+          <t>(305251175, Or  Leder: 0,-10)</t>
         </is>
       </c>
     </row>
@@ -463,14 +463,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 561.8412363853096</t>
+          <t>cost: 812.7830972132518</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 67.1051545481637</t>
+          <t>time: 98.47288715165648</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
build child's constructor from excel - in progress
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: 7,8)</t>
+          <t>(203957296, Omri Ben Shabat: -8,7)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: -8,5)</t>
+          <t>(206532695, Matan Vakrat: 8,-6)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -8,-8)</t>
+          <t>(302962915, Asher  Odeh: -8,-6)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: 6,-2)</t>
+          <t>(308035542, Anastasia  Kubi: -8,-1)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: -7,-7)</t>
+          <t>(311177802, Christina  Uksusman: 5,6)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: 0,-10)</t>
+          <t>(305251175, Or  Leder: -9,-4)</t>
         </is>
       </c>
     </row>
@@ -463,14 +463,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 812.7830972132518</t>
+          <t>cost: 834.1838832406117</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 98.47288715165648</t>
+          <t>time: 101.14798540507647</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
moving calculate_euclidean_dist to child class and build constructor from excel to child, car and school
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: -8,7)</t>
+          <t>(203957296, Omri Ben Shabat: -7,-5)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: 8,-6)</t>
+          <t>(206532695, Matan Vakrat: 1,-7)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -8,-6)</t>
+          <t>(302962915, Asher  Odeh: -7,6)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: -8,-1)</t>
+          <t>(308035542, Anastasia  Kubi: -7,-8)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: 5,6)</t>
+          <t>(311177802, Christina  Uksusman: 0,-4)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -9,-4)</t>
+          <t>(305251175, Or  Leder: -6,3)</t>
         </is>
       </c>
     </row>
@@ -463,14 +463,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 834.1838832406117</t>
+          <t>cost: 710.7430643061329</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 101.14798540507647</t>
+          <t>time: 85.7178830382666</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
moving calculate_cost_time to car class and refactor
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,32 +424,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: -7,-5)</t>
+          <t>(203957296, Omri Ben Shabat: -2,3)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: 1,-7)</t>
+          <t>(206532695, Matan Vakrat: 4,-10)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: -7,6)</t>
+          <t>(302962915, Asher  Odeh: 8,8)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: -7,-8)</t>
+          <t>(308035542, Anastasia  Kubi: -5,2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: 0,-4)</t>
+          <t>(311177802, Christina  Uksusman: 4,6)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -6,3)</t>
+          <t>(305251175, Or  Leder: -6,6)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>(308051846, Eyal  Sofer: -3,-3)</t>
         </is>
       </c>
     </row>
@@ -463,14 +468,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 710.7430643061329</t>
+          <t>cost: 670.2245000844722</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 85.7178830382666</t>
+          <t>time: 80.65306251055902</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change from dictionary to list and on progress of choose the best path
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,37 +424,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: -9,-1)</t>
+          <t>(203957296, Omri Ben Shabat: 4,1)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: -8,5)</t>
+          <t>(206532695, Matan Vakrat: -9,0)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: 5,9)</t>
+          <t>(302962915, Asher  Odeh: 0,-5)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: 7,0)</t>
+          <t>(308035542, Anastasia  Kubi: 0,-2)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: -9,6)</t>
+          <t>(311177802, Christina  Uksusman: 9,-1)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -5,-2)</t>
+          <t>(305251175, Or  Leder: -5,0)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>(308051846, Eyal  Sofer: -7,-9)</t>
+          <t>(308051846, Eyal  Sofer: -10,-9)</t>
         </is>
       </c>
     </row>
@@ -468,14 +468,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 718.9908480639502</t>
+          <t>cost: 659.0273893066587</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 86.74885600799378</t>
+          <t>time: 79.25342366333234</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finish choose the best path
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -424,37 +424,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>(203957296, Omri Ben Shabat: 4,1)</t>
+          <t>(302962915, Asher  Odeh: -9,-6)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>(206532695, Matan Vakrat: -9,0)</t>
+          <t>(305251175, Or  Leder: 2,-6)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>(302962915, Asher  Odeh: 0,-5)</t>
+          <t>(206532695, Matan Vakrat: 3,0)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(308035542, Anastasia  Kubi: 0,-2)</t>
+          <t>(203957296, Omri Ben Shabat: 1,4)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(311177802, Christina  Uksusman: 9,-1)</t>
+          <t>(308035542, Anastasia  Kubi: 0,2)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>(305251175, Or  Leder: -5,0)</t>
+          <t>(308051846, Eyal  Sofer: -5,3)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>(308051846, Eyal  Sofer: -10,-9)</t>
+          <t>(311177802, Christina  Uksusman: -7,8)</t>
         </is>
       </c>
     </row>
@@ -468,14 +468,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cost: 659.0273893066587</t>
+          <t>cost: 416.184492796085</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time: 79.25342366333234</t>
+          <t>time: 48.898061599510626</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Printing all the graphs in one graph, calculating how long each child time travel
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,32 +489,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corene  </t>
+          <t xml:space="preserve">Letha  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Myra  </t>
+          <t xml:space="preserve">Stephenie  </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>9.13,-6.03</t>
+          <t>-9.1,7.31</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Georgie(mother): 0544823581</t>
+          <t>Sibyl(mother): 0567328221</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>7:00:00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>32.0</t>
         </is>
       </c>
     </row>
@@ -526,32 +531,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nubia  </t>
+          <t xml:space="preserve">Ema  </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Royce  </t>
+          <t xml:space="preserve">Ardell  </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>9.74,-6.64</t>
+          <t>-6.44,3.18</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Augustus(father): 0517389040</t>
+          <t>Carley(grandmother): 0533587167</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7:01:00</t>
+          <t>7:06:00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>26.0</t>
         </is>
       </c>
     </row>
@@ -563,32 +573,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kandis  </t>
+          <t xml:space="preserve">Marni  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Zulma  </t>
+          <t xml:space="preserve">Shanika  </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>9.03,-3.47</t>
+          <t>-2.69,6.26</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Kylie(mother): 0575413269</t>
+          <t>Lady(mother): 0560804012</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7:05:00</t>
+          <t>7:12:00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>20.0</t>
         </is>
       </c>
     </row>
@@ -600,32 +615,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Francisca  </t>
+          <t xml:space="preserve">Alexia  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stevie  </t>
+          <t xml:space="preserve">Ramonita  </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5.29,-1.7</t>
+          <t>-2.83,7.67</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Bernardine(mother): 0561339273</t>
+          <t>Han(father): 0567537032</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>7:10:00</t>
+          <t>7:14:00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>18.0</t>
         </is>
       </c>
     </row>
@@ -637,32 +657,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Marni  </t>
+          <t xml:space="preserve">Jeanine  </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shanika  </t>
+          <t xml:space="preserve">Janee  </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5.85,-3.16</t>
+          <t>-1.93,9.03</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Lady(mother): 0560804012</t>
+          <t>Teresa(mother): 0517627420</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7:13:00</t>
+          <t>7:16:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>16.0</t>
         </is>
       </c>
     </row>
@@ -674,32 +699,37 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alexia  </t>
+          <t xml:space="preserve">Frankie  </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ramonita  </t>
+          <t xml:space="preserve">Flavia  </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.22,-4.99</t>
+          <t>3.22,4.01</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Han(father): 0567537032</t>
+          <t>Cyrus(mother): 0522363358</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7:18:00</t>
+          <t>7:26:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>6.0</t>
         </is>
       </c>
     </row>
@@ -736,7 +766,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7:26:00</t>
+          <t>7:32:00</t>
         </is>
       </c>
     </row>
@@ -760,7 +790,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>26.0</t>
+          <t>32.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the color of school points to yellow
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -489,27 +489,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ema  </t>
+          <t xml:space="preserve">Frankie  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ardell  </t>
+          <t xml:space="preserve">Flavia  </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-9.79,-8.09</t>
+          <t>9.96,8.49</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Carley(grandmother): 0533587167</t>
+          <t>Cyrus(mother): 0522363358</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>37.0</t>
+          <t>30.0</t>
         </is>
       </c>
     </row>
@@ -531,37 +531,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Trudie  </t>
+          <t xml:space="preserve">Collette  </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fleta  </t>
+          <t xml:space="preserve">Billi  </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-4.18,-8.88</t>
+          <t>9.82,6.59</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Anneliese(father): 0548973345</t>
+          <t>Elias(mother): 0578741979</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7:07:00</t>
+          <t>7:03:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>27.0</t>
         </is>
       </c>
     </row>
@@ -573,37 +573,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alexia  </t>
+          <t xml:space="preserve">Britta  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ramonita  </t>
+          <t xml:space="preserve">Jamel  </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-1.65,-8.14</t>
+          <t>5.79,5.55</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Han(father): 0567537032</t>
+          <t>Albertine(father): 0574981040</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7:11:00</t>
+          <t>7:08:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>26.0</t>
+          <t>22.0</t>
         </is>
       </c>
     </row>
@@ -615,32 +615,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corene  </t>
+          <t xml:space="preserve">Lorinda  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Myra  </t>
+          <t xml:space="preserve">Tyron  </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4.52,-9.26</t>
+          <t>8.07,2.26</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Georgie(mother): 0544823581</t>
+          <t>Teresa(grandmother): 0558587699</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>7:20:00</t>
+          <t>7:13:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -657,140 +657,98 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Marni  </t>
+          <t xml:space="preserve">Corene  </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shanika  </t>
+          <t xml:space="preserve">Myra  </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5.4,-6.02</t>
+          <t>8.46,-1.79</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Lady(mother): 0560804012</t>
+          <t>Georgie(mother): 0544823581</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7:24:00</t>
+          <t>7:19:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>11.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elwanda  </t>
+          <t>Ironiah</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cassy  </t>
+          <t>mySchool</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-1.98,-2.1</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tamisha(mother): 0550693864</t>
+          <t>Shir(secretary): 0523345098</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7:34:00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>3.0</t>
+          <t>7:30:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>cost</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Ironiah</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>mySchool</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Shir(secretary): 0523345098</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>7:37:00</t>
+          <t>25</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cost</t>
+          <t>time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>25</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>37.0</t>
+          <t>30.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the color of school points to yellow, Match the colors in all the graphs
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>9.96,8.49</t>
+          <t>-0.18,-7.37</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>32.0</t>
         </is>
       </c>
     </row>
@@ -531,27 +531,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Collette  </t>
+          <t>Ron</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Billi  </t>
+          <t>Cohen</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>9.82,6.59</t>
+          <t>-2.33,-7.05</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Elias(mother): 0578741979</t>
+          <t>Bernardine(mother): 0576270618</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>27.0</t>
+          <t>29.0</t>
         </is>
       </c>
     </row>
@@ -573,27 +573,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Britta  </t>
+          <t xml:space="preserve">Alexia  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jamel  </t>
+          <t xml:space="preserve">Ramonita  </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5.79,5.55</t>
+          <t>-5.15,-3.61</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Albertine(father): 0574981040</t>
+          <t>Han(father): 0567537032</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>24.0</t>
         </is>
       </c>
     </row>
@@ -615,27 +615,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lorinda  </t>
+          <t xml:space="preserve">Randolph  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tyron  </t>
+          <t xml:space="preserve">Bridgette  </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>8.07,2.26</t>
+          <t>-9.16,-4.56</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Teresa(grandmother): 0558587699</t>
+          <t>Lenny(father): 0505536740</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>19.0</t>
         </is>
       </c>
     </row>
@@ -657,98 +657,266 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corene  </t>
+          <t xml:space="preserve">Britta  </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Myra  </t>
+          <t xml:space="preserve">Jamel  </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>8.46,-1.79</t>
+          <t>-6.72,-1.52</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Georgie(mother): 0544823581</t>
+          <t>Albertine(father): 0574981040</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7:19:00</t>
+          <t>7:18:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>14.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ironiah</t>
+          <t xml:space="preserve">Francisca  </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>mySchool</t>
+          <t xml:space="preserve">Stevie  </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-7.14,-1.26</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Shir(secretary): 0523345098</t>
+          <t>Bernardine(mother): 0561339273</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7:30:00</t>
+          <t>7:19:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>13.0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cost</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Demetra  </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Francene  </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-6.3,-0.62</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Dorian(mother): 0534328089</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>7:21:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>11.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Collette  </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Billi  </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-4.83,-1.02</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Elias(mother): 0578741979</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>7:24:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patti  </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lavenia  </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-0.63,-1.53</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Jennell(mother): 0503029941</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>7:29:00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>school</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ironiah</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>mySchool</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Shir(secretary): 0523345098</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>7:32:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>cost</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>time</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>30.0</t>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>32.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug of histogram fix
</commit_message>
<xml_diff>
--- a/Groups0.xlsx
+++ b/Groups0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -489,27 +489,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elwanda  </t>
+          <t xml:space="preserve">Collette  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cassy  </t>
+          <t xml:space="preserve">Billi  </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6.83,8.21</t>
+          <t>-6,9</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Tamisha(mother): 0550693864</t>
+          <t>Elias(mother): 0578741979</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -531,37 +531,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Britta  </t>
+          <t xml:space="preserve">Lorinda  </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jamel  </t>
+          <t xml:space="preserve">Tyron  </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6.21,6.64</t>
+          <t>-7,8</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Albertine(father): 0574981040</t>
+          <t>Teresa(grandmother): 0558587699</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7:03:00</t>
+          <t>7:02:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>18.0</t>
         </is>
       </c>
     </row>
@@ -573,37 +573,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Randolph  </t>
+          <t xml:space="preserve">Lorinda  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bridgette  </t>
+          <t xml:space="preserve">Tyron  </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3.91,7.01</t>
+          <t>-7,8</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Lenny(father): 0505536740</t>
+          <t>Teresa(grandmother): 0558587699</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7:07:00</t>
+          <t>7:02:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>18.0</t>
         </is>
       </c>
     </row>
@@ -615,96 +615,180 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Patti  </t>
+          <t xml:space="preserve">Jeanine  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lavenia  </t>
+          <t xml:space="preserve">Janee  </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4.35,1.93</t>
+          <t>-7,7</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Jennell(mother): 0503029941</t>
+          <t>Teresa(mother): 0517627420</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>7:14:00</t>
+          <t>7:04:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>16.0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>school</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ironiah</t>
+          <t>Ron</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>mySchool</t>
+          <t>Cohen</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-8,7</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Shir(secretary): 0523345098</t>
+          <t>Bernardine(mother): 0576270618</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7:20:00</t>
+          <t>7:06:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>14.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cost</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nubia  </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Royce  </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-9,7</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Augustus(father): 0517389040</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>7:08:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>12.0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>school</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ironiah</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>mySchool</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Shir(secretary): 0523345098</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>7:20:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cost</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>65.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>time</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>20.0</t>
         </is>

</xml_diff>